<commit_message>
Before Experiment under Left Edge Outflow Condition
</commit_message>
<xml_diff>
--- a/data/input/guideForParameterInput.xlsx
+++ b/data/input/guideForParameterInput.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="179">
   <si>
     <t>[m/Myr]</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -393,9 +393,6 @@
     <t>모의 결과를 출력하는 실행 간격</t>
   </si>
   <si>
-    <t>모델 영역으로부터 유출이 발생한는 유출구 또는 경계 조건. 0, 하나의 유출구, 1, 아래의 경계면, 2, 위 아래 경계면, 4, 모든 경계면.</t>
-  </si>
-  <si>
     <t>외곽 경계 고도 조건. 0: 고도 (inf) 고정. 1: 경동성 요곡 지반융기운동 모의시 영서쪽 외곽 경계</t>
   </si>
   <si>
@@ -571,6 +568,15 @@
   </si>
   <si>
     <t>[m^2-2mfa*pfa S^-2mfa*pfa]</t>
+  </si>
+  <si>
+    <t>INIT_ELEV_20140403T194139.txt</t>
+  </si>
+  <si>
+    <t>[m/Myr]</t>
+  </si>
+  <si>
+    <t>모델 영역으로부터 유출이 발생한는 유출구 또는 경계 조건. 0: 하나의 유출구(mid bottom). 1: 아래의 경계면. 2: 위 아래 경계면. 3: 하나의 유출구(left edge) 4, 모든 경계면.</t>
   </si>
 </sst>
 </file>
@@ -710,7 +716,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -723,8 +729,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -812,8 +824,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -885,8 +906,26 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -917,9 +956,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -927,9 +963,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
@@ -1031,8 +1064,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -1044,6 +1104,9 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1056,6 +1119,9 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
@@ -2131,10 +2197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2142,1176 +2208,1191 @@
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="3.5" customWidth="1"/>
-    <col min="7" max="7" width="57.6640625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="57.6640625" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" thickBot="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="22" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" thickTop="1" thickBot="1">
+      <c r="A2" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="47">
+        <v>1</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="46" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="20" thickTop="1" thickBot="1">
-      <c r="A2" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="10">
+      <c r="F2" s="43"/>
+      <c r="G2" s="33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18">
+      <c r="A3" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="10">
+        <v>100</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18">
+      <c r="A4" s="18"/>
+      <c r="B4" s="11">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="11">
+        <v>100</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19" thickBot="1">
+      <c r="A5" s="19"/>
+      <c r="B5" s="12">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="12">
+        <v>25</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18">
+      <c r="A6" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="13">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18">
+      <c r="A7" s="18"/>
+      <c r="B7" s="48">
+        <v>6</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18">
+      <c r="A8" s="18"/>
+      <c r="B8" s="14">
+        <v>7</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19" thickBot="1">
+      <c r="A9" s="19"/>
+      <c r="B9" s="15">
+        <v>8</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18">
+      <c r="A10" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="49">
+        <v>9</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="49">
+        <v>500000</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18">
+      <c r="A11" s="18"/>
+      <c r="B11" s="14">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="21">
+        <v>1</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18">
+      <c r="A12" s="18"/>
+      <c r="B12" s="14">
+        <v>11</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="14">
+        <v>2</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18">
+      <c r="A13" s="18"/>
+      <c r="B13" s="14">
+        <v>12</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="14">
+        <f>E10/E14</f>
+        <v>10000</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19" thickBot="1">
+      <c r="A14" s="19"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="41">
+        <v>50</v>
+      </c>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:7" ht="18">
+      <c r="A15" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="13">
+        <v>13</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18">
+      <c r="A16" s="18"/>
+      <c r="B16" s="14">
+        <v>14</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="21">
+        <v>0</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18">
+      <c r="A17" s="18"/>
+      <c r="B17" s="14">
+        <v>15</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18">
+      <c r="A18" s="18"/>
+      <c r="B18" s="50">
+        <v>16</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="50">
+        <f>(E10*E12)*E19</f>
+        <v>1000</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18">
+      <c r="A19" s="18"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="51">
+        <f>E20*0.000001</f>
+        <v>1E-3</v>
+      </c>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="18">
+      <c r="A20" s="18"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="E20" s="52">
+        <v>1000</v>
+      </c>
+      <c r="F20" s="23"/>
+    </row>
+    <row r="21" spans="1:7" ht="18">
+      <c r="A21" s="18"/>
+      <c r="B21" s="26">
+        <v>17</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="26">
+        <v>0</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18">
+      <c r="A22" s="18"/>
+      <c r="B22" s="14">
+        <v>18</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="27">
+        <v>0</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18">
+      <c r="A23" s="18"/>
+      <c r="B23" s="14">
         <v>19</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18">
-      <c r="A3" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="11">
-        <v>2</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="C23" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="27">
+        <v>0</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18">
+      <c r="A24" s="18"/>
+      <c r="B24" s="25">
         <v>20</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="11">
-        <v>100</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="35" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="20"/>
-      <c r="B4" s="12">
-        <v>3</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="12">
-        <v>100</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="19" thickBot="1">
-      <c r="A5" s="21"/>
-      <c r="B5" s="13">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="13">
-        <v>25</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18">
-      <c r="A6" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="15">
-        <v>5</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="15">
-        <v>1</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="35" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="20"/>
-      <c r="B7" s="16">
-        <v>6</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="18">
-      <c r="A8" s="20"/>
-      <c r="B8" s="16">
-        <v>7</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="23">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19" thickBot="1">
-      <c r="A9" s="21"/>
-      <c r="B9" s="17">
-        <v>8</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="35" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18">
-      <c r="A10" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="15">
-        <v>9</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="15">
-        <v>10000</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="18">
-      <c r="A11" s="20"/>
-      <c r="B11" s="16">
-        <v>10</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="23">
-        <v>1</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="35" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="18">
-      <c r="A12" s="20"/>
-      <c r="B12" s="16">
-        <v>11</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="16">
-        <v>2</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="35" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="18">
-      <c r="A13" s="20"/>
-      <c r="B13" s="16">
-        <v>12</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="16">
-        <v>200</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="35" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="19" thickBot="1">
-      <c r="A14" s="21"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="43">
-        <f>E10/E13</f>
-        <v>50</v>
-      </c>
-      <c r="F14" s="24"/>
-    </row>
-    <row r="15" spans="1:7" ht="18">
-      <c r="A15" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="15">
-        <v>13</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="18">
-      <c r="A16" s="20"/>
-      <c r="B16" s="16">
-        <v>14</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="23">
-        <v>0</v>
-      </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="18">
-      <c r="A17" s="20"/>
-      <c r="B17" s="16">
-        <v>15</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="23">
-        <v>0</v>
-      </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="35" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18">
-      <c r="A18" s="20"/>
-      <c r="B18" s="26">
-        <v>16</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="26">
-        <v>4</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18">
-      <c r="A19" s="20"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" s="40">
-        <f>E18/(E10*E12)</f>
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="1:7" ht="18">
-      <c r="A20" s="20"/>
-      <c r="B20" s="28">
-        <v>17</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="28">
-        <v>0</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18">
-      <c r="A21" s="20"/>
-      <c r="B21" s="16">
-        <v>18</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="29">
-        <v>0</v>
-      </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="35" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="18">
-      <c r="A22" s="20"/>
-      <c r="B22" s="16">
-        <v>19</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="29">
-        <v>0</v>
-      </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="35" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="18">
-      <c r="A23" s="20"/>
-      <c r="B23" s="27">
-        <v>20</v>
-      </c>
-      <c r="C23" s="30" t="s">
+      <c r="C24" s="28" t="s">
         <v>40</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="30">
-        <v>0</v>
-      </c>
-      <c r="F23" s="29"/>
-      <c r="G23" s="35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18">
-      <c r="A24" s="20"/>
-      <c r="B24" s="28">
-        <v>21</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>41</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>82</v>
       </c>
       <c r="E24" s="28">
+        <v>0</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18">
+      <c r="A25" s="18"/>
+      <c r="B25" s="26">
+        <v>21</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="26">
         <v>1</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="35" t="s">
+      <c r="F25" s="14"/>
+      <c r="G25" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18">
+      <c r="A26" s="18"/>
+      <c r="B26" s="14">
+        <v>22</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="27">
+        <v>0</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="33" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18">
-      <c r="A25" s="20"/>
-      <c r="B25" s="16">
-        <v>22</v>
-      </c>
-      <c r="C25" s="29" t="s">
+    <row r="27" spans="1:7" ht="18">
+      <c r="A27" s="18"/>
+      <c r="B27" s="14">
+        <v>23</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18">
+      <c r="A28" s="18"/>
+      <c r="B28" s="25">
+        <v>24</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="27"/>
+      <c r="G28" s="33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18">
+      <c r="A29" s="18"/>
+      <c r="B29" s="14">
+        <v>25</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="27">
+        <v>0</v>
+      </c>
+      <c r="F29" s="27"/>
+      <c r="G29" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="19" thickBot="1">
+      <c r="A30" s="19"/>
+      <c r="B30" s="15">
+        <v>26</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="29">
+        <v>0</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18">
+      <c r="A31" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="13">
+        <v>27</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="13">
+        <v>1.4E-5</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18">
+      <c r="A32" s="18"/>
+      <c r="B32" s="14">
+        <v>28</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="35">
+        <v>3.5199999999999999E-4</v>
+      </c>
+      <c r="F32" s="34"/>
+      <c r="G32" s="33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18">
+      <c r="A33" s="18"/>
+      <c r="B33" s="14">
+        <v>29</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="35">
+        <v>5.1599999999999997E-4</v>
+      </c>
+      <c r="F33" s="34"/>
+      <c r="G33" s="33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="19" thickBot="1">
+      <c r="A34" s="19"/>
+      <c r="B34" s="15">
+        <v>30</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18">
+      <c r="A35" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="13">
+        <v>31</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="13">
+        <v>2E-3</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="18">
+      <c r="A36" s="18"/>
+      <c r="B36" s="14">
+        <v>32</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="F36" s="21"/>
+      <c r="G36" s="33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="19" thickBot="1">
+      <c r="A37" s="19"/>
+      <c r="B37" s="15">
+        <v>33</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F37" s="14"/>
+      <c r="G37" s="33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18">
+      <c r="A38" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="13">
+        <v>34</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="18">
+      <c r="A39" s="18"/>
+      <c r="B39" s="14">
+        <v>35</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="F39" s="14"/>
+      <c r="G39" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18">
+      <c r="A40" s="18"/>
+      <c r="B40" s="50">
+        <v>36</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40" s="50">
+        <v>25</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18">
+      <c r="A41" s="18"/>
+      <c r="B41" s="48">
+        <v>37</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="48">
+        <v>0.75</v>
+      </c>
+      <c r="F41" s="21"/>
+      <c r="G41" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18">
+      <c r="A42" s="18"/>
+      <c r="B42" s="24">
+        <v>38</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="31">
+        <v>3600</v>
+      </c>
+      <c r="F42" s="21"/>
+      <c r="G42" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18">
+      <c r="A43" s="18"/>
+      <c r="B43" s="14">
+        <v>39</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="21">
+        <v>1</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="G43" s="33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="18">
+      <c r="A44" s="18"/>
+      <c r="B44" s="14">
+        <v>40</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="21">
+        <v>1</v>
+      </c>
+      <c r="F44" s="14"/>
+      <c r="G44" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18">
+      <c r="A45" s="18"/>
+      <c r="B45" s="24">
+        <v>41</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" s="24">
+        <v>5</v>
+      </c>
+      <c r="F45" s="14"/>
+      <c r="G45" s="33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="18">
+      <c r="A46" s="18"/>
+      <c r="B46" s="14">
         <v>42</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="C46" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="29">
-        <v>0</v>
-      </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="18">
-      <c r="A26" s="20"/>
-      <c r="B26" s="16">
-        <v>23</v>
-      </c>
-      <c r="C26" s="29" t="s">
+      <c r="E46" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="F46" s="14"/>
+      <c r="G46" s="33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="18">
+      <c r="A47" s="18"/>
+      <c r="B47" s="14">
         <v>43</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="29">
-        <v>0</v>
-      </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="18">
-      <c r="A27" s="20"/>
-      <c r="B27" s="27">
-        <v>24</v>
-      </c>
-      <c r="C27" s="30" t="s">
+      <c r="C47" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="21">
+        <v>0.53</v>
+      </c>
+      <c r="F47" s="14"/>
+      <c r="G47" s="33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="19" thickBot="1">
+      <c r="A48" s="19"/>
+      <c r="B48" s="15">
         <v>44</v>
       </c>
-      <c r="D27" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="30">
-        <v>0</v>
-      </c>
-      <c r="F27" s="29"/>
-      <c r="G27" s="35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="18">
-      <c r="A28" s="20"/>
-      <c r="B28" s="16">
-        <v>25</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="29">
-        <v>0</v>
-      </c>
-      <c r="F28" s="29"/>
-      <c r="G28" s="35" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="19" thickBot="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="17">
-        <v>26</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" s="31">
-        <v>0</v>
-      </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="18">
-      <c r="A30" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="15">
-        <v>27</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="15">
-        <v>1.4E-5</v>
-      </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18">
-      <c r="A31" s="20"/>
-      <c r="B31" s="16">
-        <v>28</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="37">
-        <v>3.5199999999999999E-4</v>
-      </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="35" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="18">
-      <c r="A32" s="20"/>
-      <c r="B32" s="16">
-        <v>29</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="37">
-        <v>5.1599999999999997E-4</v>
-      </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="19" thickBot="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="17">
-        <v>30</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E33" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="F33" s="16"/>
-      <c r="G33" s="35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="18">
-      <c r="A34" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="15">
-        <v>31</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="15">
-        <v>2E-3</v>
-      </c>
-      <c r="F34" s="16"/>
-      <c r="G34" s="35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18">
-      <c r="A35" s="20"/>
-      <c r="B35" s="16">
-        <v>32</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="23">
-        <v>0.3</v>
-      </c>
-      <c r="F35" s="23"/>
-      <c r="G35" s="35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="19" thickBot="1">
-      <c r="A36" s="21"/>
-      <c r="B36" s="17">
-        <v>33</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="17">
-        <v>0.6</v>
-      </c>
-      <c r="F36" s="16"/>
-      <c r="G36" s="35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="18">
-      <c r="A37" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="15">
-        <v>34</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="15">
-        <v>1.2</v>
-      </c>
-      <c r="F37" s="16"/>
-      <c r="G37" s="35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="18">
-      <c r="A38" s="20"/>
-      <c r="B38" s="16">
-        <v>35</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" s="16">
-        <v>0.6</v>
-      </c>
-      <c r="F38" s="16"/>
-      <c r="G38" s="35" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="18">
-      <c r="A39" s="20"/>
-      <c r="B39" s="26">
-        <v>36</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" s="26">
-        <v>25</v>
-      </c>
-      <c r="F39" s="16"/>
-      <c r="G39" s="35" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="18">
-      <c r="A40" s="20"/>
-      <c r="B40" s="16">
-        <v>37</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E40" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="F40" s="23"/>
-      <c r="G40" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="18">
-      <c r="A41" s="20"/>
-      <c r="B41" s="26">
-        <v>38</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="33">
-        <v>3600</v>
-      </c>
-      <c r="F41" s="23"/>
-      <c r="G41" s="35" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="18">
-      <c r="A42" s="20"/>
-      <c r="B42" s="16">
-        <v>39</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E42" s="23">
-        <v>1</v>
-      </c>
-      <c r="F42" s="16"/>
-      <c r="G42" s="35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="18">
-      <c r="A43" s="20"/>
-      <c r="B43" s="16">
-        <v>40</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="23">
-        <v>1</v>
-      </c>
-      <c r="F43" s="16"/>
-      <c r="G43" s="35" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="18">
-      <c r="A44" s="20"/>
-      <c r="B44" s="26">
-        <v>41</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="E44" s="26">
-        <v>5</v>
-      </c>
-      <c r="F44" s="16"/>
-      <c r="G44" s="35" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="18">
-      <c r="A45" s="20"/>
-      <c r="B45" s="16">
-        <v>42</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="23">
-        <v>0.5</v>
-      </c>
-      <c r="F45" s="16"/>
-      <c r="G45" s="35" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="18">
-      <c r="A46" s="20"/>
-      <c r="B46" s="16">
-        <v>43</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E46" s="23">
-        <v>0.53</v>
-      </c>
-      <c r="F46" s="16"/>
-      <c r="G46" s="35" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="19" thickBot="1">
-      <c r="A47" s="21"/>
-      <c r="B47" s="17">
-        <v>44</v>
-      </c>
-      <c r="C47" s="17" t="s">
+      <c r="C48" s="15" t="s">
         <v>64</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E47" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="F47" s="16"/>
-      <c r="G47" s="35" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="18">
-      <c r="A48" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" s="15">
-        <v>45</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>65</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>82</v>
       </c>
       <c r="E48" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="18">
+      <c r="A49" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="13">
+        <v>45</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" s="13">
         <v>1</v>
       </c>
-      <c r="F48" s="16"/>
-      <c r="G48" s="35" t="s">
+      <c r="F49" s="14"/>
+      <c r="G49" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="18">
+      <c r="A50" s="18"/>
+      <c r="B50" s="24">
+        <v>46</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="24">
+        <v>6000</v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="33" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="18">
-      <c r="A49" s="20"/>
-      <c r="B49" s="26">
-        <v>46</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="D49" s="26" t="s">
+    <row r="51" spans="1:7" ht="18">
+      <c r="A51" s="18"/>
+      <c r="B51" s="14">
+        <v>47</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" s="21">
+        <v>10</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="18">
+      <c r="A52" s="18"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="26">
-        <v>6000</v>
-      </c>
-      <c r="F49" s="16"/>
-      <c r="G49" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="18">
-      <c r="A50" s="20"/>
-      <c r="B50" s="16">
-        <v>47</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="16" t="s">
+      <c r="E52" s="39">
+        <f>E51*E5^2</f>
+        <v>6250</v>
+      </c>
+      <c r="F52" s="32"/>
+    </row>
+    <row r="53" spans="1:7" ht="18">
+      <c r="A53" s="18"/>
+      <c r="B53" s="24">
+        <v>48</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="23">
-        <v>10</v>
-      </c>
-      <c r="F50" s="16"/>
-      <c r="G50" s="35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="18">
-      <c r="A51" s="20"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="39" t="s">
+      <c r="E53" s="24">
+        <v>1.8</v>
+      </c>
+      <c r="F53" s="14"/>
+      <c r="G53" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="D51" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" s="41">
-        <f>E50*E5^2</f>
-        <v>6250</v>
-      </c>
-      <c r="F51" s="34"/>
-    </row>
-    <row r="52" spans="1:7" ht="18">
-      <c r="A52" s="20"/>
-      <c r="B52" s="26">
-        <v>48</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="26" t="s">
+    </row>
+    <row r="54" spans="1:7" ht="18">
+      <c r="A54" s="18"/>
+      <c r="B54" s="14">
+        <v>49</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E52" s="26">
-        <v>1.8</v>
-      </c>
-      <c r="F52" s="16"/>
-      <c r="G52" s="35" t="s">
+      <c r="E54" s="21">
+        <v>2.1</v>
+      </c>
+      <c r="F54" s="14"/>
+      <c r="G54" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="18">
-      <c r="A53" s="20"/>
-      <c r="B53" s="16">
-        <v>49</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" s="16" t="s">
+    <row r="55" spans="1:7" ht="18">
+      <c r="A55" s="18"/>
+      <c r="B55" s="14">
+        <v>50</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E55" s="21">
+        <v>2650</v>
+      </c>
+      <c r="F55" s="14"/>
+      <c r="G55" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18">
+      <c r="A56" s="18"/>
+      <c r="B56" s="14">
+        <v>51</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="F56" s="14"/>
+      <c r="G56" s="33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18">
+      <c r="A57" s="18"/>
+      <c r="B57" s="14">
+        <v>52</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" s="21">
+        <v>0.4</v>
+      </c>
+      <c r="F57" s="14"/>
+      <c r="G57" s="33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18">
+      <c r="A58" s="18"/>
+      <c r="B58" s="25">
+        <v>53</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="F58" s="14"/>
+      <c r="G58" s="33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="18">
+      <c r="A59" s="18"/>
+      <c r="B59" s="24">
+        <v>54</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="E53" s="23">
-        <v>2.1</v>
-      </c>
-      <c r="F53" s="16"/>
-      <c r="G53" s="35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="18">
-      <c r="A54" s="20"/>
-      <c r="B54" s="16">
-        <v>50</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="E54" s="23">
-        <v>2650</v>
-      </c>
-      <c r="F54" s="16"/>
-      <c r="G54" s="35" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="18">
-      <c r="A55" s="20"/>
-      <c r="B55" s="16">
-        <v>51</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="F55" s="16"/>
-      <c r="G55" s="35" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="18">
-      <c r="A56" s="20"/>
-      <c r="B56" s="16">
-        <v>52</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E56" s="23">
-        <v>0.4</v>
-      </c>
-      <c r="F56" s="16"/>
-      <c r="G56" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="18">
-      <c r="A57" s="20"/>
-      <c r="B57" s="27">
-        <v>53</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D57" s="27" t="s">
+      <c r="E59" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F59" s="14"/>
+      <c r="G59" s="33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="18">
+      <c r="A60" s="18"/>
+      <c r="B60" s="14">
+        <v>55</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E60" s="21">
+        <v>0.7</v>
+      </c>
+      <c r="F60" s="14"/>
+      <c r="G60" s="33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18">
+      <c r="A61" s="18"/>
+      <c r="B61" s="14">
+        <v>56</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="E61" s="21">
+        <v>3.1000000000000003E-11</v>
+      </c>
+      <c r="F61" s="14"/>
+      <c r="G61" s="33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="19" thickBot="1">
+      <c r="A62" s="19"/>
+      <c r="B62" s="15">
+        <v>57</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E57" s="27">
-        <v>0.03</v>
-      </c>
-      <c r="F57" s="16"/>
-      <c r="G57" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="18">
-      <c r="A58" s="20"/>
-      <c r="B58" s="26">
-        <v>54</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E58" s="26">
-        <v>0.6</v>
-      </c>
-      <c r="F58" s="16"/>
-      <c r="G58" s="35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="18">
-      <c r="A59" s="20"/>
-      <c r="B59" s="16">
-        <v>55</v>
-      </c>
-      <c r="C59" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E59" s="23">
-        <v>0.7</v>
-      </c>
-      <c r="F59" s="16"/>
-      <c r="G59" s="35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="18">
-      <c r="A60" s="20"/>
-      <c r="B60" s="16">
-        <v>56</v>
-      </c>
-      <c r="C60" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="E60" s="23">
-        <v>3.1000000000000003E-11</v>
-      </c>
-      <c r="F60" s="16"/>
-      <c r="G60" s="35" t="s">
+      <c r="E62" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="F62" s="14"/>
+      <c r="G62" s="33" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="19" thickBot="1">
-      <c r="A61" s="21"/>
-      <c r="B61" s="17">
-        <v>57</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E61" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="F61" s="16"/>
-      <c r="G61" s="35" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3342,66 +3423,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="15" thickBot="1">
-      <c r="B2" s="47" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="47" t="s">
+      <c r="B2" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="45" t="s">
         <v>170</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3">
-        <f>List!E30</f>
+        <f>List!E31</f>
         <v>1.4E-5</v>
       </c>
       <c r="D3">
-        <f>List!E31</f>
+        <f>List!E32</f>
         <v>3.5199999999999999E-4</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="15" thickBot="1">
-      <c r="B5" s="47" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" s="47" t="s">
+      <c r="B5" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="45" t="s">
         <v>172</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6">
-        <f>List!E32</f>
+        <f>List!E33</f>
         <v>5.1599999999999997E-4</v>
       </c>
       <c r="D6">
-        <f>List!E33</f>
+        <f>List!E34</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="16" thickBot="1">
-      <c r="B8" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>165</v>
+      <c r="B8" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" thickTop="1">
-      <c r="B9" s="46">
+      <c r="B9" s="44">
         <v>0</v>
       </c>
       <c r="C9">
@@ -3414,7 +3495,7 @@
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="46">
+      <c r="B10" s="44">
         <v>0.05</v>
       </c>
       <c r="C10">
@@ -3427,7 +3508,7 @@
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="46">
+      <c r="B11" s="44">
         <v>0.1</v>
       </c>
       <c r="C11">
@@ -3440,7 +3521,7 @@
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="46">
+      <c r="B12" s="44">
         <v>0.15</v>
       </c>
       <c r="C12">
@@ -3453,7 +3534,7 @@
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="46">
+      <c r="B13" s="44">
         <v>0.2</v>
       </c>
       <c r="C13">
@@ -3466,7 +3547,7 @@
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="46">
+      <c r="B14" s="44">
         <v>0.25</v>
       </c>
       <c r="C14">
@@ -3479,7 +3560,7 @@
       </c>
     </row>
     <row r="15" spans="2:4">
-      <c r="B15" s="46">
+      <c r="B15" s="44">
         <v>0.3</v>
       </c>
       <c r="C15">
@@ -3492,7 +3573,7 @@
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="46">
+      <c r="B16" s="44">
         <v>0.35</v>
       </c>
       <c r="C16">
@@ -3505,7 +3586,7 @@
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="46">
+      <c r="B17" s="44">
         <v>0.4</v>
       </c>
       <c r="C17">
@@ -3518,7 +3599,7 @@
       </c>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="46">
+      <c r="B18" s="44">
         <v>0.45</v>
       </c>
       <c r="C18">
@@ -3531,7 +3612,7 @@
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="46">
+      <c r="B19" s="44">
         <v>0.5</v>
       </c>
       <c r="C19">
@@ -3544,7 +3625,7 @@
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="46">
+      <c r="B20" s="44">
         <v>0.55000000000000004</v>
       </c>
       <c r="C20">
@@ -3557,7 +3638,7 @@
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="46">
+      <c r="B21" s="44">
         <v>0.6</v>
       </c>
       <c r="C21">
@@ -3570,7 +3651,7 @@
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="46">
+      <c r="B22" s="44">
         <v>0.65</v>
       </c>
       <c r="C22">
@@ -3583,7 +3664,7 @@
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="46">
+      <c r="B23" s="44">
         <v>0.7</v>
       </c>
       <c r="C23">
@@ -3596,7 +3677,7 @@
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="46">
+      <c r="B24" s="44">
         <v>0.75</v>
       </c>
       <c r="C24">
@@ -3609,7 +3690,7 @@
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="46">
+      <c r="B25" s="44">
         <v>0.8</v>
       </c>
       <c r="C25">
@@ -3622,7 +3703,7 @@
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="46">
+      <c r="B26" s="44">
         <v>0.85</v>
       </c>
       <c r="C26">
@@ -3635,7 +3716,7 @@
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="46">
+      <c r="B27" s="44">
         <v>0.9</v>
       </c>
       <c r="C27">
@@ -3648,7 +3729,7 @@
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="46">
+      <c r="B28" s="44">
         <v>0.95</v>
       </c>
       <c r="C28">
@@ -3661,7 +3742,7 @@
       </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" s="46">
+      <c r="B29" s="44">
         <v>1</v>
       </c>
       <c r="C29">
@@ -3674,7 +3755,7 @@
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="46">
+      <c r="B30" s="44">
         <v>1.05</v>
       </c>
       <c r="C30">
@@ -3687,7 +3768,7 @@
       </c>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="46">
+      <c r="B31" s="44">
         <v>1.1000000000000001</v>
       </c>
       <c r="C31">
@@ -3700,7 +3781,7 @@
       </c>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="46">
+      <c r="B32" s="44">
         <v>1.1499999999999999</v>
       </c>
       <c r="C32">
@@ -3713,7 +3794,7 @@
       </c>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="46">
+      <c r="B33" s="44">
         <v>1.2</v>
       </c>
       <c r="C33">
@@ -3726,7 +3807,7 @@
       </c>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="46">
+      <c r="B34" s="44">
         <v>1.25</v>
       </c>
       <c r="C34">
@@ -3739,7 +3820,7 @@
       </c>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="46">
+      <c r="B35" s="44">
         <v>1.3</v>
       </c>
       <c r="C35">
@@ -3752,7 +3833,7 @@
       </c>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="46">
+      <c r="B36" s="44">
         <v>1.35</v>
       </c>
       <c r="C36">
@@ -3765,7 +3846,7 @@
       </c>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="46">
+      <c r="B37" s="44">
         <v>1.4</v>
       </c>
       <c r="C37">
@@ -3778,7 +3859,7 @@
       </c>
     </row>
     <row r="38" spans="2:4">
-      <c r="B38" s="46">
+      <c r="B38" s="44">
         <v>1.45</v>
       </c>
       <c r="C38">
@@ -3791,7 +3872,7 @@
       </c>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39" s="46">
+      <c r="B39" s="44">
         <v>1.5</v>
       </c>
       <c r="C39">
@@ -3804,7 +3885,7 @@
       </c>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="46">
+      <c r="B40" s="44">
         <v>1.55</v>
       </c>
       <c r="C40">
@@ -3817,7 +3898,7 @@
       </c>
     </row>
     <row r="41" spans="2:4">
-      <c r="B41" s="46">
+      <c r="B41" s="44">
         <v>1.6</v>
       </c>
       <c r="C41">
@@ -3830,7 +3911,7 @@
       </c>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" s="46">
+      <c r="B42" s="44">
         <v>1.65</v>
       </c>
       <c r="C42">
@@ -3843,7 +3924,7 @@
       </c>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" s="46">
+      <c r="B43" s="44">
         <v>1.7</v>
       </c>
       <c r="C43">
@@ -3856,7 +3937,7 @@
       </c>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44" s="46">
+      <c r="B44" s="44">
         <v>1.75</v>
       </c>
       <c r="C44">
@@ -3869,7 +3950,7 @@
       </c>
     </row>
     <row r="45" spans="2:4">
-      <c r="B45" s="46">
+      <c r="B45" s="44">
         <v>1.8</v>
       </c>
       <c r="C45">
@@ -3882,7 +3963,7 @@
       </c>
     </row>
     <row r="46" spans="2:4">
-      <c r="B46" s="46">
+      <c r="B46" s="44">
         <v>1.85</v>
       </c>
       <c r="C46">
@@ -3895,7 +3976,7 @@
       </c>
     </row>
     <row r="47" spans="2:4">
-      <c r="B47" s="46">
+      <c r="B47" s="44">
         <v>1.9</v>
       </c>
       <c r="C47">
@@ -3908,7 +3989,7 @@
       </c>
     </row>
     <row r="48" spans="2:4">
-      <c r="B48" s="46">
+      <c r="B48" s="44">
         <v>1.95</v>
       </c>
       <c r="C48">
@@ -3921,7 +4002,7 @@
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="46">
+      <c r="B49" s="44">
         <v>2</v>
       </c>
       <c r="C49">

</xml_diff>

<commit_message>
commit for regular backup
</commit_message>
<xml_diff>
--- a/data/input/guideForParameterInput.xlsx
+++ b/data/input/guideForParameterInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="20480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23180" windowHeight="20480"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="2" r:id="rId1"/>
@@ -1732,11 +1732,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127434520"/>
-        <c:axId val="-2127437704"/>
+        <c:axId val="2143270680"/>
+        <c:axId val="2142673976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127434520"/>
+        <c:axId val="2143270680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -1795,12 +1795,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127437704"/>
+        <c:crossAx val="2142673976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127437704"/>
+        <c:axId val="2142673976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1858,7 +1858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127434520"/>
+        <c:crossAx val="2143270680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2200,7 +2200,7 @@
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3397,6 +3397,20 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15">
+      <formula1>"0, 1, 2, 3, 4"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E16 E17 E21">
+      <formula1>"0,1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E25">
+      <formula1>"1,2,3"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E49">
+      <formula1>"1,2"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>